<commit_message>
Improved histogram of weights
</commit_message>
<xml_diff>
--- a/results/optim_info(1).xlsx
+++ b/results/optim_info(1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\RPrograms PC\OSPC\EvaluateWtdSynFile\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE497164-4531-4150-A6C4-EFB5F51E684A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABBB9C00-B1D5-465D-B6CB-F330ABA3F9C6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" xr2:uid="{01D1F3BA-3972-4A4D-959F-286DBDDC3133}"/>
   </bookViews>
@@ -6847,13 +6847,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>390525</xdr:colOff>
+      <xdr:colOff>95250</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>57149</xdr:rowOff>
     </xdr:to>
@@ -7188,7 +7188,7 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="M35" sqref="M35"/>
+      <selection pane="bottomRight" activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>